<commit_message>
update with single HB session to lbs side to test current state
</commit_message>
<xml_diff>
--- a/TrevorHB_lb.xlsx
+++ b/TrevorHB_lb.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="241">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -716,6 +716,33 @@
   </si>
   <si>
     <t xml:space="preserve">22 Dec 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Nov 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-7.5,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.5,3,5,7,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-50,0,4,3,3,2,2,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-30,2,3,5,3,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-15,2,9,4,4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-50,2,6,5,3,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45,4,7,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-35,2,7,6,4,4</t>
   </si>
 </sst>
 </file>
@@ -737,16 +764,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -796,11 +826,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -816,18 +846,127 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.49"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2590,35 +2729,67 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="0" t="s">
+      <c r="B56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="0" t="s">
+      <c r="F56" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G56" s="0" t="s">
+      <c r="G56" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H56" s="0" t="s">
+      <c r="H56" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I56" s="0" t="s">
+      <c r="I56" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="J56" s="0" t="s">
+      <c r="J56" s="2" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>